<commit_message>
mvp feature complete: placing a batch of client orders
</commit_message>
<xml_diff>
--- a/Project0/TempMohit/Data/ShoppingLists.xlsx
+++ b/Project0/TempMohit/Data/ShoppingLists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Project0\Damle_M_Valentine_N_P0\Project0\TempMohit\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81393303-BC4D-4343-8B30-399E76BD38FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78C75CE-52E6-44DC-8B23-94EB685FCC35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrderClientRef" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>OrderId</t>
   </si>
@@ -50,6 +50,18 @@
   </si>
   <si>
     <t>milk</t>
+  </si>
+  <si>
+    <t>hat</t>
+  </si>
+  <si>
+    <t>umbrella</t>
+  </si>
+  <si>
+    <t>rain jacket</t>
+  </si>
+  <si>
+    <t>bottle</t>
   </si>
 </sst>
 </file>
@@ -367,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,6 +411,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -406,10 +426,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C50773F-024F-44B0-906C-0332C3E31ED2}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,6 +500,72 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added a GetEarliestOrderIdProcessed sequence
</commit_message>
<xml_diff>
--- a/Project0/TempMohit/Data/ShoppingLists.xlsx
+++ b/Project0/TempMohit/Data/ShoppingLists.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Project0\Damle_M_Valentine_N_P0\Project0\TempMohit\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78C75CE-52E6-44DC-8B23-94EB685FCC35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7787FAC-0DB1-43E7-8A9D-5E9C41D48787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrderClientRef" sheetId="1" r:id="rId1"/>
-    <sheet name="OrderList" sheetId="2" r:id="rId2"/>
+    <sheet name="OrderListIncoming" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>

</xml_diff>